<commit_message>
Tweak parameters for nesi
</commit_message>
<xml_diff>
--- a/data/branch_weight_data_v0-1.xlsx
+++ b/data/branch_weight_data_v0-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\McGrath\occ-coseismic\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmc753\Work\occ-coseismic\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD6E492-D733-41EF-A5B7-219E76364BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D352904-6F80-41CD-82E5-7B3825A40334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30630" yWindow="3105" windowWidth="28800" windowHeight="15600" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all sheets" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="288">
   <si>
     <t>N</t>
   </si>
@@ -901,6 +901,9 @@
   </si>
   <si>
     <t>creep</t>
+  </si>
+  <si>
+    <t>Def_weight</t>
   </si>
 </sst>
 </file>
@@ -7278,23 +7281,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C3AB27-DA22-46B6-9275-CBA251195A6D}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="5" max="10" width="12.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="19" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="5" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="11" width="12.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="19" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7314,37 +7319,40 @@
         <v>251</v>
       </c>
       <c r="G1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H1" t="s">
         <v>246</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>247</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>258</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>254</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>256</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>259</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>264</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>225</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>27.9</v>
       </c>
@@ -7364,34 +7372,37 @@
         <v>260</v>
       </c>
       <c r="G2">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
         <v>0.34233999999999998</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.48699999999999999</v>
       </c>
-      <c r="I2">
-        <f t="shared" ref="I2:I8" si="0">PRODUCT(G2:H2)</f>
-        <v>0.16671957999999998</v>
-      </c>
       <c r="J2">
+        <f>PRODUCT(G2:I2)</f>
+        <v>8.3359789999999989E-2</v>
+      </c>
+      <c r="K2">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K2">
-        <f t="shared" ref="K2:K8" si="1">J2*I2</f>
-        <v>2.126282411939925E-5</v>
-      </c>
       <c r="L2">
-        <f>K2/(SUM(K$2:K$22))</f>
+        <f t="shared" ref="L2:L8" si="0">K2*J2</f>
+        <v>1.0631412059699625E-5</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M19" si="1">L2/(SUM(L$2:L$22))</f>
         <v>8.344323323323323E-2</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>280</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>27.9</v>
       </c>
@@ -7411,34 +7422,37 @@
         <v>260</v>
       </c>
       <c r="G3">
+        <v>0.5</v>
+      </c>
+      <c r="H3">
         <v>0.34233999999999998</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.255</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3" si="2">PRODUCT(G3:H3)</f>
-        <v>8.7296699999999991E-2</v>
-      </c>
       <c r="J3">
+        <f t="shared" ref="J3:J19" si="2">PRODUCT(G3:I3)</f>
+        <v>4.3648349999999995E-2</v>
+      </c>
+      <c r="K3">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3" si="3">J3*I3</f>
-        <v>1.1133511602560182E-5</v>
-      </c>
       <c r="L3">
-        <f>K3/(SUM(K$2:K$22))</f>
+        <f t="shared" ref="L3" si="3">K3*J3</f>
+        <v>5.5667558012800908E-6</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="1"/>
         <v>4.3692042042042037E-2</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>280</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>27.9</v>
       </c>
@@ -7458,34 +7472,37 @@
         <v>260</v>
       </c>
       <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
         <v>0.34233999999999998</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.25700000000000001</v>
       </c>
-      <c r="I4">
-        <f t="shared" ref="I4" si="4">PRODUCT(G4:H4)</f>
-        <v>8.7981379999999998E-2</v>
-      </c>
       <c r="J4">
+        <f t="shared" si="2"/>
+        <v>4.3990689999999999E-2</v>
+      </c>
+      <c r="K4">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K4">
-        <f t="shared" ref="K4" si="5">J4*I4</f>
-        <v>1.1220833262188106E-5</v>
-      </c>
       <c r="L4">
-        <f>K4/(SUM(K$2:K$22))</f>
+        <f t="shared" ref="L4" si="4">K4*J4</f>
+        <v>5.6104166310940532E-6</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="1"/>
         <v>4.4034724724724729E-2</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>280</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>21.5</v>
       </c>
@@ -7505,34 +7522,37 @@
         <v>260</v>
       </c>
       <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5">
         <v>0.45212999999999998</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.48699999999999999</v>
       </c>
-      <c r="I5">
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>0.11009365499999998</v>
+      </c>
+      <c r="K5">
+        <v>1.27536454442839E-4</v>
+      </c>
+      <c r="L5">
         <f t="shared" si="0"/>
-        <v>0.22018730999999997</v>
-      </c>
-      <c r="J5">
-        <v>1.27536454442839E-4</v>
-      </c>
-      <c r="K5">
+        <v>1.4040954415353132E-5</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="1"/>
-        <v>2.8081908830706263E-5</v>
-      </c>
-      <c r="L5">
-        <f>K5/(SUM(K$2:K$22))</f>
         <v>0.11020385885885885</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>279</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>21.5</v>
       </c>
@@ -7552,34 +7572,37 @@
         <v>260</v>
       </c>
       <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
         <v>0.45212999999999998</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.255</v>
       </c>
-      <c r="I6">
-        <f t="shared" ref="I6:I7" si="6">PRODUCT(G6:H6)</f>
-        <v>0.11529315</v>
-      </c>
       <c r="J6">
+        <f t="shared" si="2"/>
+        <v>5.7646574999999999E-2</v>
+      </c>
+      <c r="K6">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K6">
-        <f t="shared" ref="K6:K7" si="7">J6*I6</f>
-        <v>1.4704079572546403E-5</v>
-      </c>
       <c r="L6">
-        <f>K6/(SUM(K$2:K$22))</f>
+        <f t="shared" ref="L6:L7" si="5">K6*J6</f>
+        <v>7.3520397862732014E-6</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
         <v>5.7704279279279284E-2</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>279</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>21.5</v>
       </c>
@@ -7599,34 +7622,37 @@
         <v>260</v>
       </c>
       <c r="G7">
+        <v>0.5</v>
+      </c>
+      <c r="H7">
         <v>0.45212999999999998</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.25700000000000001</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="6"/>
-        <v>0.11619741</v>
-      </c>
       <c r="J7">
+        <f t="shared" si="2"/>
+        <v>5.8098705E-2</v>
+      </c>
+      <c r="K7">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="7"/>
-        <v>1.4819405686840885E-5</v>
-      </c>
       <c r="L7">
-        <f>K7/(SUM(K$2:K$22))</f>
+        <f t="shared" si="5"/>
+        <v>7.4097028434204424E-6</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
         <v>5.8156861861861864E-2</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>279</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>16.5</v>
       </c>
@@ -7646,34 +7672,37 @@
         <v>260</v>
       </c>
       <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8">
         <v>0.20552999999999999</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.48699999999999999</v>
       </c>
-      <c r="I8">
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>5.0046555E-2</v>
+      </c>
+      <c r="K8">
+        <v>1.27536454442839E-4</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="0"/>
-        <v>0.10009311</v>
-      </c>
-      <c r="J8">
-        <v>1.27536454442839E-4</v>
-      </c>
-      <c r="K8">
+        <v>6.3827601817785363E-6</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="1"/>
-        <v>1.2765520363557073E-5</v>
-      </c>
-      <c r="L8">
-        <f>K8/(SUM(K$2:K$22))</f>
         <v>5.0096651651651655E-2</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>278</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16.5</v>
       </c>
@@ -7693,34 +7722,37 @@
         <v>260</v>
       </c>
       <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9">
         <v>0.20552999999999999</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.255</v>
       </c>
-      <c r="I9">
-        <f t="shared" ref="I9:I10" si="8">PRODUCT(G9:H9)</f>
-        <v>5.2410149999999996E-2</v>
-      </c>
       <c r="J9">
+        <f t="shared" si="2"/>
+        <v>2.6205074999999998E-2</v>
+      </c>
+      <c r="K9">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K9">
-        <f t="shared" ref="K9:K10" si="9">J9*I9</f>
-        <v>6.6842047078173577E-6</v>
-      </c>
       <c r="L9">
-        <f>K9/(SUM(K$2:K$22))</f>
+        <f t="shared" ref="L9:L10" si="6">K9*J9</f>
+        <v>3.3421023539086788E-6</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
         <v>2.6231306306306306E-2</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>278</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>16.5</v>
       </c>
@@ -7740,34 +7772,37 @@
         <v>260</v>
       </c>
       <c r="G10">
+        <v>0.5</v>
+      </c>
+      <c r="H10">
         <v>0.20552999999999999</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.25700000000000001</v>
       </c>
-      <c r="I10">
-        <f t="shared" si="8"/>
-        <v>5.282121E-2</v>
-      </c>
       <c r="J10">
+        <f t="shared" si="2"/>
+        <v>2.6410605E-2</v>
+      </c>
+      <c r="K10">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K10">
-        <f t="shared" si="9"/>
-        <v>6.736629842780632E-6</v>
-      </c>
       <c r="L10">
-        <f>K10/(SUM(K$2:K$22))</f>
+        <f t="shared" si="6"/>
+        <v>3.368314921390316E-6</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
         <v>2.6437042042042044E-2</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>278</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>27.9</v>
       </c>
@@ -7787,34 +7822,37 @@
         <v>260</v>
       </c>
       <c r="G11">
+        <v>0.5</v>
+      </c>
+      <c r="H11">
         <v>0.34233999999999998</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.48699999999999999</v>
       </c>
-      <c r="I11">
-        <f t="shared" ref="I11:I17" si="10">PRODUCT(G11:H11)</f>
-        <v>0.16671957999999998</v>
-      </c>
       <c r="J11">
+        <f t="shared" si="2"/>
+        <v>8.3359789999999989E-2</v>
+      </c>
+      <c r="K11">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K11">
-        <f t="shared" ref="K11:K17" si="11">J11*I11</f>
-        <v>2.126282411939925E-5</v>
-      </c>
       <c r="L11">
-        <f>K11/(SUM(K$2:K$22))</f>
+        <f t="shared" ref="L11:L17" si="7">K11*J11</f>
+        <v>1.0631412059699625E-5</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
         <v>8.344323323323323E-2</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>277</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>27.9</v>
       </c>
@@ -7834,34 +7872,37 @@
         <v>260</v>
       </c>
       <c r="G12">
+        <v>0.5</v>
+      </c>
+      <c r="H12">
         <v>0.34233999999999998</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>0.255</v>
       </c>
-      <c r="I12">
-        <f t="shared" ref="I12:I13" si="12">PRODUCT(G12:H12)</f>
-        <v>8.7296699999999991E-2</v>
-      </c>
       <c r="J12">
+        <f t="shared" si="2"/>
+        <v>4.3648349999999995E-2</v>
+      </c>
+      <c r="K12">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K12">
-        <f t="shared" ref="K12:K13" si="13">J12*I12</f>
-        <v>1.1133511602560182E-5</v>
-      </c>
       <c r="L12">
-        <f>K12/(SUM(K$2:K$22))</f>
+        <f t="shared" ref="L12:L13" si="8">K12*J12</f>
+        <v>5.5667558012800908E-6</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
         <v>4.3692042042042037E-2</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>277</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>27.9</v>
       </c>
@@ -7881,34 +7922,37 @@
         <v>260</v>
       </c>
       <c r="G13">
+        <v>0.5</v>
+      </c>
+      <c r="H13">
         <v>0.34233999999999998</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>0.25700000000000001</v>
       </c>
-      <c r="I13">
-        <f t="shared" si="12"/>
-        <v>8.7981379999999998E-2</v>
-      </c>
       <c r="J13">
+        <f t="shared" si="2"/>
+        <v>4.3990689999999999E-2</v>
+      </c>
+      <c r="K13">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K13">
-        <f t="shared" si="13"/>
-        <v>1.1220833262188106E-5</v>
-      </c>
       <c r="L13">
-        <f>K13/(SUM(K$2:K$22))</f>
+        <f t="shared" si="8"/>
+        <v>5.6104166310940532E-6</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
         <v>4.4034724724724729E-2</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>277</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>21.5</v>
       </c>
@@ -7928,34 +7972,37 @@
         <v>260</v>
       </c>
       <c r="G14">
+        <v>0.5</v>
+      </c>
+      <c r="H14">
         <v>0.45212999999999998</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.48699999999999999</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="10"/>
-        <v>0.22018730999999997</v>
-      </c>
       <c r="J14">
+        <f t="shared" si="2"/>
+        <v>0.11009365499999998</v>
+      </c>
+      <c r="K14">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K14">
-        <f t="shared" si="11"/>
-        <v>2.8081908830706263E-5</v>
-      </c>
       <c r="L14">
-        <f>K14/(SUM(K$2:K$22))</f>
+        <f t="shared" si="7"/>
+        <v>1.4040954415353132E-5</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
         <v>0.11020385885885885</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>281</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>21.5</v>
       </c>
@@ -7975,34 +8022,37 @@
         <v>260</v>
       </c>
       <c r="G15">
+        <v>0.5</v>
+      </c>
+      <c r="H15">
         <v>0.45212999999999998</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>0.255</v>
       </c>
-      <c r="I15">
-        <f t="shared" ref="I15:I16" si="14">PRODUCT(G15:H15)</f>
-        <v>0.11529315</v>
-      </c>
       <c r="J15">
+        <f t="shared" si="2"/>
+        <v>5.7646574999999999E-2</v>
+      </c>
+      <c r="K15">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K15">
-        <f t="shared" ref="K15:K16" si="15">J15*I15</f>
-        <v>1.4704079572546403E-5</v>
-      </c>
       <c r="L15">
-        <f>K15/(SUM(K$2:K$22))</f>
+        <f t="shared" ref="L15:L16" si="9">K15*J15</f>
+        <v>7.3520397862732014E-6</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
         <v>5.7704279279279284E-2</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>281</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>21.5</v>
       </c>
@@ -8022,34 +8072,37 @@
         <v>260</v>
       </c>
       <c r="G16">
+        <v>0.5</v>
+      </c>
+      <c r="H16">
         <v>0.45212999999999998</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>0.25700000000000001</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="14"/>
-        <v>0.11619741</v>
-      </c>
       <c r="J16">
+        <f t="shared" si="2"/>
+        <v>5.8098705E-2</v>
+      </c>
+      <c r="K16">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="15"/>
-        <v>1.4819405686840885E-5</v>
-      </c>
       <c r="L16">
-        <f>K16/(SUM(K$2:K$22))</f>
+        <f t="shared" si="9"/>
+        <v>7.4097028434204424E-6</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
         <v>5.8156861861861864E-2</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>281</v>
       </c>
-      <c r="N16" t="s">
+      <c r="O16" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16.5</v>
       </c>
@@ -8069,34 +8122,37 @@
         <v>260</v>
       </c>
       <c r="G17">
+        <v>0.5</v>
+      </c>
+      <c r="H17">
         <v>0.20552999999999999</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>0.48699999999999999</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="10"/>
-        <v>0.10009311</v>
-      </c>
       <c r="J17">
+        <f t="shared" si="2"/>
+        <v>5.0046555E-2</v>
+      </c>
+      <c r="K17">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K17">
-        <f t="shared" si="11"/>
-        <v>1.2765520363557073E-5</v>
-      </c>
       <c r="L17">
-        <f>K17/(SUM(K$2:K$22))</f>
+        <f t="shared" si="7"/>
+        <v>6.3827601817785363E-6</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
         <v>5.0096651651651655E-2</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>282</v>
       </c>
-      <c r="N17" t="s">
+      <c r="O17" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16.5</v>
       </c>
@@ -8116,34 +8172,37 @@
         <v>260</v>
       </c>
       <c r="G18">
+        <v>0.5</v>
+      </c>
+      <c r="H18">
         <v>0.20552999999999999</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>0.255</v>
       </c>
-      <c r="I18">
-        <f t="shared" ref="I18:I19" si="16">PRODUCT(G18:H18)</f>
-        <v>5.2410149999999996E-2</v>
-      </c>
       <c r="J18">
+        <f t="shared" si="2"/>
+        <v>2.6205074999999998E-2</v>
+      </c>
+      <c r="K18">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K18">
-        <f t="shared" ref="K18:K19" si="17">J18*I18</f>
-        <v>6.6842047078173577E-6</v>
-      </c>
       <c r="L18">
-        <f>K18/(SUM(K$2:K$22))</f>
+        <f t="shared" ref="L18:L19" si="10">K18*J18</f>
+        <v>3.3421023539086788E-6</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
         <v>2.6231306306306306E-2</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>282</v>
       </c>
-      <c r="N18" t="s">
+      <c r="O18" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16.5</v>
       </c>
@@ -8163,30 +8222,33 @@
         <v>260</v>
       </c>
       <c r="G19">
+        <v>0.5</v>
+      </c>
+      <c r="H19">
         <v>0.20552999999999999</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>0.25700000000000001</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="16"/>
-        <v>5.282121E-2</v>
-      </c>
       <c r="J19">
+        <f t="shared" si="2"/>
+        <v>2.6410605E-2</v>
+      </c>
+      <c r="K19">
         <v>1.27536454442839E-4</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="17"/>
-        <v>6.736629842780632E-6</v>
-      </c>
       <c r="L19">
-        <f>K19/(SUM(K$2:K$22))</f>
+        <f t="shared" si="10"/>
+        <v>3.368314921390316E-6</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
         <v>2.6437042042042044E-2</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>282</v>
       </c>
-      <c r="N19" t="s">
+      <c r="O19" t="s">
         <v>285</v>
       </c>
     </row>

</xml_diff>